<commit_message>
Revise figure size and include repository and archival information.
</commit_message>
<xml_diff>
--- a/Analysis results/FSCI2022_Ranking results.xlsx
+++ b/Analysis results/FSCI2022_Ranking results.xlsx
@@ -17,10 +17,10 @@
     <t xml:space="preserve">Indicator</t>
   </si>
   <si>
-    <t xml:space="preserve">Worst Ranking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Best Ranking</t>
+    <t xml:space="preserve">Bottom Ranking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Top Ranking</t>
   </si>
   <si>
     <t xml:space="preserve">Cost of healthy diet</t>

</xml_diff>